<commit_message>
final touches and documentation
</commit_message>
<xml_diff>
--- a/Results sheet.xlsx
+++ b/Results sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefanoskonstantinou/Documents/Zurich/year2/NLP Essentials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefanoskonstantinou/Documents/Zurich/year2/NLP-Domain-Adaptation-Exploration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C833DD81-4C6F-7840-AFC2-E087888681BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B37C11-2CAD-F941-B092-2102C38F1BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16220" xr2:uid="{4470D931-4829-5145-9D7B-AE15E4DAA536}"/>
   </bookViews>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="17">
-  <si>
-    <t>Dataset size</t>
-  </si>
-  <si>
-    <t>Twitter</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
   <si>
     <t>ACC</t>
   </si>
@@ -86,13 +80,25 @@
     <t>HeFiT</t>
   </si>
   <si>
-    <t>Reddit</t>
+    <t>Dataset size: 1500 Reddit Data</t>
+  </si>
+  <si>
+    <t>Dataset size: 3750 Reddit Data</t>
+  </si>
+  <si>
+    <t>Dataset size: 3750 Twitter Data</t>
+  </si>
+  <si>
+    <t>Dataset size: 1500 Twitter Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -208,22 +214,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,7 +554,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -551,807 +564,838 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11">
-        <v>1500</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
-      <c r="H1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="11">
-        <v>3750</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="12"/>
+      <c r="A1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="8"/>
+      <c r="H1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2">
+        <v>6</v>
+      </c>
+      <c r="B3" s="9">
         <v>0.69730000000000003</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="9">
         <v>0.69740000000000002</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="9">
         <v>4.3099999999999999E-2</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="9">
         <v>0.69730000000000003</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="10">
         <v>0.70030000000000003</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="2">
+      <c r="G3" s="11"/>
+      <c r="H3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="9">
         <v>0.80559999999999998</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="9">
         <v>0.80589999999999995</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="9">
         <v>5.4000000000000003E-3</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="9">
         <v>0.80559999999999998</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="10">
         <v>0.81210000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5">
+        <v>5</v>
+      </c>
+      <c r="B4" s="11">
         <v>0.75860000000000005</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="11">
         <v>0.75890000000000002</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="11">
         <v>2.9399999999999999E-2</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="11">
         <v>0.75870000000000004</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="13">
         <v>0.76400000000000001</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="13">
+      <c r="G4" s="11"/>
+      <c r="H4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="11">
         <v>0.78</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="11">
         <v>0.77959999999999996</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="11">
         <v>2.7699999999999999E-2</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="11">
         <v>0.78</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="13">
         <v>0.78800000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5">
+        <v>7</v>
+      </c>
+      <c r="B5" s="11">
         <v>0.74729999999999996</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="11">
         <v>0.74850000000000005</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="11">
         <v>3.9800000000000002E-2</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="11">
         <v>0.74729999999999996</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="13">
         <v>0.75590000000000002</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="13">
+      <c r="G5" s="11"/>
+      <c r="H5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="11">
         <v>0.8085</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="11">
         <v>0.80900000000000005</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="11">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="11">
         <v>0.8085</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="13">
         <v>0.81769999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="8">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="15">
         <v>0.65869999999999995</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="15">
         <v>0.65210000000000001</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="15">
         <v>0.1167</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="15">
         <v>0.65869999999999995</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="16">
         <v>0.67379999999999995</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="14">
+      <c r="G6" s="11"/>
+      <c r="H6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="15">
         <v>0.81730000000000003</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="15">
         <v>0.81810000000000005</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="15">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="15">
         <v>0.81810000000000005</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="16">
         <v>0.81730000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="5">
+        <v>9</v>
+      </c>
+      <c r="B7" s="11">
         <v>0.68069999999999997</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="11">
         <v>0.6804</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="11">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="11">
         <v>0.68069999999999997</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="13">
         <v>0.68520000000000003</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="13">
+      <c r="G7" s="11"/>
+      <c r="H7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="11">
         <v>0.76849999999999996</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="11">
         <v>0.76829999999999998</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="11">
         <v>1.4E-2</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="11">
         <v>0.76849999999999996</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="13">
         <v>0.77869999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="5">
+        <v>10</v>
+      </c>
+      <c r="B8" s="11">
         <v>0.68869999999999998</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="11">
         <v>0.68869999999999998</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="11">
         <v>3.1600000000000003E-2</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="11">
         <v>0.68869999999999998</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="13">
         <v>0.69199999999999995</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="13">
+      <c r="G8" s="11"/>
+      <c r="H8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="11">
         <v>0.77090000000000003</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="11">
         <v>0.77110000000000001</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="11">
         <v>1.54E-2</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="11">
         <v>0.77090000000000003</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="13">
         <v>0.78210000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="11">
+        <v>0.66930000000000001</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0.66979999999999995</v>
+      </c>
+      <c r="D9" s="11">
+        <v>3.6499999999999998E-2</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.66930000000000001</v>
+      </c>
+      <c r="F9" s="13">
+        <v>0.67620000000000002</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0.76370000000000005</v>
+      </c>
+      <c r="J9" s="11">
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="K9" s="11">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0.76370000000000005</v>
+      </c>
+      <c r="M9" s="13">
+        <v>0.77400000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="15">
+        <v>0.6613</v>
+      </c>
+      <c r="C10" s="15">
+        <v>0.66080000000000005</v>
+      </c>
+      <c r="D10" s="15">
+        <v>2.76E-2</v>
+      </c>
+      <c r="E10" s="15">
+        <v>0.6613</v>
+      </c>
+      <c r="F10" s="16">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="G10" s="11"/>
+      <c r="H10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="15">
+        <v>0.7752</v>
+      </c>
+      <c r="J10" s="15">
+        <v>0.77529999999999999</v>
+      </c>
+      <c r="K10" s="15">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="L10" s="15">
+        <v>0.76519999999999999</v>
+      </c>
+      <c r="M10" s="16">
+        <v>0.78800000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="5">
-        <v>0.66930000000000001</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0.66979999999999995</v>
-      </c>
-      <c r="D9" s="5">
-        <v>3.6499999999999998E-2</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.66930000000000001</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0.67620000000000002</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="B11" s="15">
+        <v>0.67869999999999997</v>
+      </c>
+      <c r="C11" s="15">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="D11" s="15">
+        <v>2.7300000000000001E-2</v>
+      </c>
+      <c r="E11" s="15">
+        <v>0.67869999999999997</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0.68640000000000001</v>
+      </c>
+      <c r="G11" s="11"/>
+      <c r="H11" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="13">
-        <v>0.76370000000000005</v>
-      </c>
-      <c r="J9" s="13">
-        <v>0.76359999999999995</v>
-      </c>
-      <c r="K9" s="13">
-        <v>7.4000000000000003E-3</v>
-      </c>
-      <c r="L9" s="13">
-        <v>0.76370000000000005</v>
-      </c>
-      <c r="M9" s="6">
-        <v>0.77400000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="I11" s="15">
+        <v>0.79149999999999998</v>
+      </c>
+      <c r="J11" s="15">
+        <v>0.79149999999999998</v>
+      </c>
+      <c r="K11" s="15">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="L11" s="15">
+        <v>0.79149999999999998</v>
+      </c>
+      <c r="M11" s="16">
+        <v>0.80020000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+    </row>
+    <row r="13" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+    </row>
+    <row r="14" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="8">
-        <v>0.6613</v>
-      </c>
-      <c r="C10" s="8">
-        <v>0.66080000000000005</v>
-      </c>
-      <c r="D10" s="8">
-        <v>2.76E-2</v>
-      </c>
-      <c r="E10" s="8">
-        <v>0.6613</v>
-      </c>
-      <c r="F10" s="9">
-        <v>0.66449999999999998</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="14">
-        <v>0.7752</v>
-      </c>
-      <c r="J10" s="14">
-        <v>0.77529999999999999</v>
-      </c>
-      <c r="K10" s="14">
-        <v>7.4000000000000003E-3</v>
-      </c>
-      <c r="L10" s="14">
-        <v>0.76519999999999999</v>
-      </c>
-      <c r="M10" s="9">
-        <v>0.78800000000000003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="8">
-        <v>0.67869999999999997</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0.67900000000000005</v>
-      </c>
-      <c r="D11" s="8">
-        <v>2.7300000000000001E-2</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0.67869999999999997</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0.68640000000000001</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="8">
-        <v>0.79149999999999998</v>
-      </c>
-      <c r="J11" s="8">
-        <v>0.79149999999999998</v>
-      </c>
-      <c r="K11" s="8">
-        <v>1.6400000000000001E-2</v>
-      </c>
-      <c r="L11" s="8">
-        <v>0.79149999999999998</v>
-      </c>
-      <c r="M11" s="9">
-        <v>0.80020000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="11">
-        <v>1500</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="H14" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" s="11">
-        <v>3750</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="12"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="19"/>
     </row>
     <row r="15" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="E15" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="F15" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="2" t="s">
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="L15" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="M15" s="10" t="s">
         <v>4</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="2">
+        <v>6</v>
+      </c>
+      <c r="B16" s="9">
         <v>0.62929999999999997</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="9">
         <v>0.62929999999999997</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="9">
         <v>4.5600000000000002E-2</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="9">
         <v>0.62929999999999997</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="10">
         <v>0.64439999999999997</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="2">
+      <c r="G16" s="11"/>
+      <c r="H16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="9">
         <v>0.81889999999999996</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="9">
         <v>0.81889999999999996</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="9">
         <v>3.2399999999999998E-2</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="9">
         <v>0.81889999999999996</v>
       </c>
-      <c r="M16" s="3">
+      <c r="M16" s="10">
         <v>0.82020000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="5">
+        <v>5</v>
+      </c>
+      <c r="B17" s="11">
         <v>0.67869999999999997</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="11">
         <v>0.67820000000000003</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="11">
         <v>2.1499999999999998E-2</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="11">
         <v>0.67869999999999997</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="13">
         <v>0.69869999999999999</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I17" s="13">
+      <c r="G17" s="11"/>
+      <c r="H17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="11">
         <v>0.84960000000000002</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="11">
         <v>0.84970000000000001</v>
       </c>
-      <c r="K17" s="13">
+      <c r="K17" s="11">
         <v>1.37E-2</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="11">
         <v>0.84960000000000002</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M17" s="13">
         <v>0.85119999999999996</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="5">
+        <v>7</v>
+      </c>
+      <c r="B18" s="11">
         <v>0.69199999999999995</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="11">
         <v>0.69159999999999999</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="11">
         <v>1.6799999999999999E-2</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="11">
         <v>0.69199999999999995</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="13">
         <v>0.70679999999999998</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="13">
+      <c r="G18" s="11"/>
+      <c r="H18" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="11">
         <v>0.84419999999999995</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="11">
         <v>0.84460000000000002</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="11">
         <v>1.2200000000000001E-2</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="11">
         <v>0.84419999999999995</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M18" s="13">
         <v>0.84760000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="8">
+      <c r="A19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="15">
         <v>0.67269999999999996</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="15">
         <v>0.67459999999999998</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="15">
         <v>3.5900000000000001E-2</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="15">
         <v>0.67269999999999996</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="16">
         <v>0.69840000000000002</v>
       </c>
-      <c r="H19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" s="14">
+      <c r="G19" s="11"/>
+      <c r="H19" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="15">
         <v>0.85070000000000001</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="15">
         <v>0.85099999999999998</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K19" s="15">
         <v>7.9000000000000008E-3</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="15">
         <v>0.85060000000000002</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M19" s="16">
         <v>0.85309999999999997</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="5">
+        <v>9</v>
+      </c>
+      <c r="B20" s="11">
         <v>0.61799999999999999</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="11">
         <v>0.61699999999999999</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="11">
         <v>1.8100000000000002E-2</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="11">
         <v>0.61799999999999999</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="13">
         <v>0.62990000000000002</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="13">
+      <c r="G20" s="11"/>
+      <c r="H20" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="11">
         <v>0.81140000000000001</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="11">
         <v>0.81179999999999997</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K20" s="11">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="11">
         <v>0.8115</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="13">
         <v>0.81410000000000005</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="13">
+        <v>10</v>
+      </c>
+      <c r="B21" s="11">
         <v>0.60599999999999998</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="11">
         <v>0.60509999999999997</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="11">
         <v>1.55E-2</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="11">
         <v>0.60599999999999998</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="13">
         <v>0.61599999999999999</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I21" s="13">
+      <c r="G21" s="11"/>
+      <c r="H21" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="11">
         <v>0.81910000000000005</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="11">
         <v>0.81969999999999998</v>
       </c>
-      <c r="K21" s="13">
+      <c r="K21" s="11">
         <v>1.15E-2</v>
       </c>
-      <c r="L21" s="13">
+      <c r="L21" s="11">
         <v>0.81920000000000004</v>
       </c>
-      <c r="M21" s="6">
+      <c r="M21" s="13">
         <v>0.82240000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="11">
+        <v>0.61929999999999996</v>
+      </c>
+      <c r="C22" s="11">
+        <v>0.61839999999999995</v>
+      </c>
+      <c r="D22" s="11">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="E22" s="11">
+        <v>0.61929999999999996</v>
+      </c>
+      <c r="F22" s="13">
+        <v>0.62529999999999997</v>
+      </c>
+      <c r="G22" s="11"/>
+      <c r="H22" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="11">
+        <v>0.80940000000000001</v>
+      </c>
+      <c r="J22" s="11">
+        <v>0.80979999999999996</v>
+      </c>
+      <c r="K22" s="11">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="L22" s="11">
+        <v>0.80940000000000001</v>
+      </c>
+      <c r="M22" s="13">
+        <v>0.8115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="15">
+        <v>0.62</v>
+      </c>
+      <c r="C23" s="15">
+        <v>0.61950000000000005</v>
+      </c>
+      <c r="D23" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="E23" s="15">
+        <v>0.62</v>
+      </c>
+      <c r="F23" s="16">
+        <v>0.69869999999999999</v>
+      </c>
+      <c r="G23" s="11"/>
+      <c r="H23" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="15">
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="J23" s="15">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="K23" s="15">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="L23" s="15">
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="M23" s="16">
+        <v>0.81689999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="13">
-        <v>0.61929999999999996</v>
-      </c>
-      <c r="C22" s="13">
-        <v>0.61839999999999995</v>
-      </c>
-      <c r="D22" s="13">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="E22" s="13">
-        <v>0.61929999999999996</v>
-      </c>
-      <c r="F22" s="6">
-        <v>0.62529999999999997</v>
-      </c>
-      <c r="H22" s="4" t="s">
+      <c r="B24" s="15">
+        <v>0.66269999999999996</v>
+      </c>
+      <c r="C24" s="15">
+        <v>0.66310000000000002</v>
+      </c>
+      <c r="D24" s="15">
+        <v>2.3599999999999999E-2</v>
+      </c>
+      <c r="E24" s="15">
+        <v>0.66269999999999996</v>
+      </c>
+      <c r="F24" s="16">
+        <v>0.67420000000000002</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="13">
-        <v>0.80940000000000001</v>
-      </c>
-      <c r="J22" s="13">
-        <v>0.80979999999999996</v>
-      </c>
-      <c r="K22" s="13">
-        <v>1.5900000000000001E-2</v>
-      </c>
-      <c r="L22" s="13">
-        <v>0.80940000000000001</v>
-      </c>
-      <c r="M22" s="6">
-        <v>0.8115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="8">
-        <v>0.62</v>
-      </c>
-      <c r="C23" s="8">
-        <v>0.61950000000000005</v>
-      </c>
-      <c r="D23" s="8">
-        <v>1E-3</v>
-      </c>
-      <c r="E23" s="8">
-        <v>0.62</v>
-      </c>
-      <c r="F23" s="9">
-        <v>0.69869999999999999</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" s="14">
-        <v>0.81440000000000001</v>
-      </c>
-      <c r="J23" s="14">
-        <v>0.81499999999999995</v>
-      </c>
-      <c r="K23" s="14">
-        <v>9.2999999999999992E-3</v>
-      </c>
-      <c r="L23" s="14">
-        <v>0.81440000000000001</v>
-      </c>
-      <c r="M23" s="9">
-        <v>0.81689999999999996</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="8">
-        <v>0.66269999999999996</v>
-      </c>
-      <c r="C24" s="8">
-        <v>0.66310000000000002</v>
-      </c>
-      <c r="D24" s="8">
-        <v>2.3599999999999999E-2</v>
-      </c>
-      <c r="E24" s="8">
-        <v>0.66269999999999996</v>
-      </c>
-      <c r="F24" s="9">
-        <v>0.67420000000000002</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="8">
+      <c r="I24" s="15">
         <v>0.83250000000000002</v>
       </c>
-      <c r="J24" s="8">
+      <c r="J24" s="15">
         <v>0.83309999999999995</v>
       </c>
-      <c r="K24" s="8">
+      <c r="K24" s="15">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="L24" s="8">
+      <c r="L24" s="15">
         <v>0.83250000000000002</v>
       </c>
-      <c r="M24" s="9">
+      <c r="M24" s="16">
         <v>0.83499999999999996</v>
       </c>
     </row>

</xml_diff>